<commit_message>
TEST for Demo.without Weight
</commit_message>
<xml_diff>
--- a/data/user_data/seoulbikeinfo_test.xlsx
+++ b/data/user_data/seoulbikeinfo_test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="322">
   <si>
     <t xml:space="preserve">구명</t>
   </si>
@@ -145,82 +145,847 @@
     <t xml:space="preserve">127.034508</t>
   </si>
   <si>
-    <t xml:space="preserve">ST-791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2306</t>
-  </si>
-  <si>
-    <t xml:space="preserve">압구정역 2번 출구 옆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">서울특별시 강남구 압구정로 지하 172압구정역 2번 출구 옆</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.527122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.028717</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST-792</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2307</t>
-  </si>
-  <si>
-    <t xml:space="preserve">압구정 한양 3차 아파트</t>
-  </si>
-  <si>
-    <t xml:space="preserve">서울특별시 강남구 압구정로 321압구정 한양 3차 아파트</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.528614</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.038559</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST-793</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">압구정파출소 앞</t>
-  </si>
-  <si>
-    <t xml:space="preserve">서울특별시 강남구 압구정로 311압구정파출소 앞</t>
+    <t xml:space="preserve">ST-1364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">자곡사거리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 밤고개로 206자곡사거리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.476028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.105942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2385</t>
+  </si>
+  <si>
+    <t xml:space="preserve">학동역</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 학동로 지하 180학동역</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.51395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.030151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sk 동우주유소 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 봉은사로 지하 201sk 동우주유소 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.509586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.040909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2387</t>
+  </si>
+  <si>
+    <t xml:space="preserve">래미안강남힐즈 사거리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 자곡로 101래미안강남힐즈 사거리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.472454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.096077</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1433</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2388</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강남구 도시관리공단</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 삼성로 628강남구 도시관리공단</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.516785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.051613</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">경기여자고등학교 후문 (삼성로3길 입구)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 개포로 지하 420경기여자고등학교 후문 (삼성로3길 입구)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.48616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.067238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1560</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">구룡마을 입구 (래미안블레스티지 아파트)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 양재대로 478구룡마을 입구 (래미안블레스티지 아파트)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.479568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.064774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">구룡초사거리 (현대아파트10동 앞 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 개포로 30310동 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.481384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.053917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-958</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">국립국악중,고교 정문 맞은편</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 논현로10길 29국립국악중,고교 정문 맞은편</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.475605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.050377</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-956</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">도곡1동 주민센터 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 도곡로 205도곡1동 주민센터 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.492809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.041389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2361</t>
+  </si>
+  <si>
+    <t xml:space="preserve">압구정역 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 신사동 580-7압구정역 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.526844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.028259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">신사동 가로수길 입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 신사동 501-5신사동 가로수길 입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.517635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.022453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2363</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강남 을지병원 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 도산대로 172 강남 을지병원 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.51918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.027466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">영동3교 북단(우성캐릭터 앞 보도)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 언주로 118영동3교 북단(우성캐릭터 앞 보도)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.485741</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.051048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2398</t>
+  </si>
+  <si>
+    <t xml:space="preserve">더라움</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 언주로 564더라움</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.50811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.039452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">밀알학교 입구 (삼성서울병원 입구)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 일원로 90밀알학교 입구 (삼성서울병원 입구)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.486561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.082672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">공무원연금매점 교차로 (개포주공9단지 입구)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 영동대로4길 10공무원연금매점 교차로 (개포주공9단지 입구)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.48872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.074539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">대모산입구역 4번 출구 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 개포로 지하 522대모산입구역 4번 출구 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.49181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.073158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">청담공원앞 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 학동로 지하 346청담공원앞 교차로</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.518711</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.05085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">논현동 광명빌딩 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 도산대로 138논현동 광명빌딩 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.51757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.023643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">역삼서초삼성 세무서 앞 (역삼빌딩 앞)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 강남대로 지하 396역삼.서초.삼성 세무서 앞 (역삼빌딩 앞)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.49847</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.030113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2408</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강남한양수자인아파트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강남구 자곡로 260강남한양수자인아파트</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
-    <t xml:space="preserve">37.529301</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.035599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST-783</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2309</t>
-  </si>
-  <si>
-    <t xml:space="preserve">청담역(우리들병원 앞)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">서울특별시 강남구 학동로 443강남구 청담동 77-76 (학동로 443 앞 도로)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.518902</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.049385</t>
+    <t xml:space="preserve">37.477341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.113274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강동구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">광진교 남단 사거리(디지털프라자앞)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 구천면로 171376 남단사거리</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.541805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.124718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-486</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">해공공원(천호동)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 올림픽로 702265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.545219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.125916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강동구청역 1번 출입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 올림픽로 지하 5501번 출입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.530773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.120926</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강동구평생학습관앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 고덕로 295명일동 320-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.5508</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.142624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-499</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">샛마을 근린공원</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 구천면로 431-2샛마을 근린공원</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.550079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.146912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">해뜨는 주유소옆 리엔파크 109동앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 상일로 152강일동 607-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.559399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.171158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-501</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">맥도날드(길동)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 천호대로 1207맥도날드(길동)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.535473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.145172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-830</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">둔촌 주공 GS 맞은편</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 양재대로 1330둔촌동 541-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.524681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.135406</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">다성이즈빌아파트(호원대 대각선 맞은편)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 성내로 91다성이즈빌아파트(호원대 대각선 맞은편)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.526825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.130028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-503</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강동경찰서</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 성내로 57강동경찰서</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.52829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.126801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강일동 리슈빌 빌딩앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 아리수로 419강일동 306-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.564301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.17395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-505</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">길동 사거리(초소앞)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 양재대로 1441성내동 379-41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.533764</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.138031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">한국종합기술사옥 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 상일동 504 상일동 삼성엔지니어링 앞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.549999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.17469</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고덕동 아남아파트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 고덕동 673고덕동 아남아파트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.557991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.144707</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고덕동 래미안 힐스테이트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 고덕동 603고덕동 래미안 힐스테이트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.561909</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.150749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고덕역 4번출구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 명일동 46-5고덕역 4번출구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.555016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.155273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고덕동 주양쇼핑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 명일동 48-2고덕동 주양쇼핑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.551998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.153297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강일 6단지</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강일동 448-2강일 6단지</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.562588</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.177612</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강일 다솜 어린이 공원</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강일동 333-2강일 다솜 어린이 공원</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.568668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.174797</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">고덕초등학교</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 고덕동 215고덕초등학교</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.561279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.167801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">동부기업(둔촌동)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 진황도로 172동부기업</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.531013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.142365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1371</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1049</t>
+  </si>
+  <si>
+    <t xml:space="preserve">강일동 10단지 아파트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 고덕로97길 20강일동 10단지 아파트</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.56118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.180267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">둔촌역 3번 출입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 양재대로 1355둔촌역 3번 출입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.526695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.135529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST-1421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">양지시장 (용성약국앞) 입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">서울특별시 강동구 고덕로 109양지시장 (용성약국앞) 입구</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.554829</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.137321</t>
   </si>
 </sst>
 </file>
@@ -235,6 +1000,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK JP Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -346,17 +1112,17 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="49:52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="24.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="10.77"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -382,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -408,7 +1174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -434,7 +1200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -460,7 +1226,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -486,7 +1252,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -512,7 +1278,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -529,65 +1295,65 @@
         <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,28 +1361,1131 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
+      <c r="D11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="1046984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1047000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>